<commit_message>
Updated format for ORT Grant report and added PDF
</commit_message>
<xml_diff>
--- a/Reports/Eugene_ORTGrantSummary_2025-12-04.xlsx
+++ b/Reports/Eugene_ORTGrantSummary_2025-12-04.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uoecs-my.sharepoint.com/personal/sethm_uoecs_org/Documents/Personal/EOE/repos/eugene-oregon/Reports/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="5" documentId="8_{D045D36E-F6C0-4B8E-9F54-A5F8A086D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{933B741C-2B7E-4D33-951D-EAB19A3E4EC2}"/>
+  <xr:revisionPtr revIDLastSave="93" documentId="8_{D045D36E-F6C0-4B8E-9F54-A5F8A086D4C6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{10593F5F-1C9D-4C4B-8ABD-3A919BAA152F}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="65145" yWindow="360" windowWidth="21600" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Data" sheetId="4" r:id="rId1"/>
@@ -183,6 +183,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -190,6 +191,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -218,7 +220,7 @@
     </font>
     <font>
       <b/>
-      <sz val="16"/>
+      <sz val="18"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -226,7 +228,7 @@
     </font>
     <font>
       <b/>
-      <sz val="18"/>
+      <sz val="22"/>
       <color theme="1"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
@@ -371,14 +373,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="44">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="44" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
@@ -418,9 +419,19 @@
     <xf numFmtId="44" fontId="2" fillId="2" borderId="6" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="4" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="44" fontId="2" fillId="2" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="14" fontId="1" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -2818,7 +2829,7 @@
           <c:order val="0"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$22</c:f>
+              <c:f>Data!$A$63</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2862,7 +2873,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$17:$F$17</c:f>
+              <c:f>Data!$B$58:$F$58</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -2885,7 +2896,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$22:$F$22</c:f>
+              <c:f>Data!$B$63:$F$63</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -2932,7 +2943,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$23</c:f>
+              <c:f>Data!$A$64</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2986,7 +2997,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$17:$F$17</c:f>
+              <c:f>Data!$B$58:$F$58</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3009,7 +3020,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$23:$F$23</c:f>
+              <c:f>Data!$B$64:$F$64</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3056,7 +3067,7 @@
           <c:order val="2"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$24</c:f>
+              <c:f>Data!$A$65</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3090,7 +3101,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$17:$F$17</c:f>
+              <c:f>Data!$B$58:$F$58</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3113,7 +3124,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$24:$F$24</c:f>
+              <c:f>Data!$B$65:$F$65</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3146,7 +3157,7 @@
           <c:order val="3"/>
           <c:tx>
             <c:strRef>
-              <c:f>Data!$A$25</c:f>
+              <c:f>Data!$A$66</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -3180,7 +3191,7 @@
           </c:dLbls>
           <c:cat>
             <c:strRef>
-              <c:f>Data!$B$17:$F$17</c:f>
+              <c:f>Data!$B$58:$F$58</c:f>
               <c:strCache>
                 <c:ptCount val="5"/>
                 <c:pt idx="0">
@@ -3203,7 +3214,7 @@
           </c:cat>
           <c:val>
             <c:numRef>
-              <c:f>Data!$B$25:$F$25</c:f>
+              <c:f>Data!$B$66:$F$66</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="5"/>
@@ -3345,7 +3356,7 @@
                     </a:solidFill>
                     <a:latin typeface="+mn-lt"/>
                   </a:rPr>
-                  <a:t>Arrests</a:t>
+                  <a:t>Actions</a:t>
                 </a:r>
               </a:p>
             </c:rich>
@@ -5480,12 +5491,12 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>142875</xdr:colOff>
-      <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>15</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6086475" cy="2667000"/>
+    <xdr:ext cx="6762750" cy="5162550"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 1" title="Chart">
@@ -5513,12 +5524,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>7</xdr:col>
-      <xdr:colOff>152399</xdr:colOff>
-      <xdr:row>13</xdr:row>
-      <xdr:rowOff>180975</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>66</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="6105525" cy="2667000"/>
+    <xdr:ext cx="6772274" cy="6229351"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="4" name="Chart 2" title="Chart">
@@ -5552,11 +5563,11 @@
   <xdr:oneCellAnchor>
     <xdr:from>
       <xdr:col>0</xdr:col>
-      <xdr:colOff>9525</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5753100" cy="2667000"/>
+    <xdr:ext cx="6762750" cy="3009900"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1226801955" name="Chart 3" title="Chart">
@@ -5582,12 +5593,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>28575</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>0</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>62</xdr:row>
+      <xdr:rowOff>190499</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5753100" cy="2667000"/>
+    <xdr:ext cx="6743700" cy="4124325"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="1940648434" name="Chart 4" title="Chart">
@@ -5613,12 +5624,12 @@
   </xdr:oneCellAnchor>
   <xdr:oneCellAnchor>
     <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>19050</xdr:colOff>
-      <xdr:row>7</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>85724</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5753100" cy="2667000"/>
+    <xdr:ext cx="6734174" cy="3971925"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 3" title="Chart">
@@ -5651,7 +5662,7 @@
       <xdr:row>7</xdr:row>
       <xdr:rowOff>9525</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5753100" cy="2667000"/>
+    <xdr:ext cx="6762750" cy="3219450"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 3" title="Chart">
@@ -5687,9 +5698,9 @@
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>9525</xdr:rowOff>
+      <xdr:rowOff>9524</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5753100" cy="2667000"/>
+    <xdr:ext cx="6705600" cy="3533775"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 3" title="Chart">
@@ -5719,10 +5730,10 @@
     <xdr:from>
       <xdr:col>0</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>19</xdr:row>
-      <xdr:rowOff>57150</xdr:rowOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="5753100" cy="2667000"/>
+    <xdr:ext cx="6705600" cy="3324225"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="3" name="Chart 3" title="Chart">
@@ -5776,8 +5787,8 @@
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{20C5EB77-878B-4CE4-8101-D361C1CDAAFF}" name="Outcomes" displayName="Outcomes" ref="A17:G25" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
-  <autoFilter ref="A17:G25" xr:uid="{20C5EB77-878B-4CE4-8101-D361C1CDAAFF}">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{20C5EB77-878B-4CE4-8101-D361C1CDAAFF}" name="Outcomes" displayName="Outcomes" ref="A58:G66" totalsRowShown="0" headerRowDxfId="54" headerRowBorderDxfId="53" tableBorderDxfId="52" totalsRowBorderDxfId="51">
+  <autoFilter ref="A58:G66" xr:uid="{20C5EB77-878B-4CE4-8101-D361C1CDAAFF}">
     <filterColumn colId="0" hiddenButton="1"/>
     <filterColumn colId="1" hiddenButton="1"/>
     <filterColumn colId="2" hiddenButton="1"/>
@@ -5815,22 +5826,22 @@
   <tableColumns count="7">
     <tableColumn id="1" xr3:uid="{886AD75C-C1E9-498D-90A9-B02309768868}" name="Metrics" dataDxfId="39"/>
     <tableColumn id="2" xr3:uid="{D8921FFA-7951-49F0-A8FD-97A89A53E0CF}" name="Q1" dataDxfId="38">
-      <calculatedColumnFormula>B$22/B$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>B$63/B$14*100000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="3" xr3:uid="{806FA61A-443C-4439-9DD9-CA7C87E28238}" name="Q2" dataDxfId="37">
-      <calculatedColumnFormula>C$22/C$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>C$63/C$14*100000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{6EB30613-04AC-4859-8872-9FE08077B60D}" name="Q3" dataDxfId="36">
-      <calculatedColumnFormula>D$22/D$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>D$63/D$14*100000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="5" xr3:uid="{B509EBBA-0C2F-45F5-A953-BDC3AB497ED8}" name="Q4" dataDxfId="35">
-      <calculatedColumnFormula>E$22/E$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>E$63/E$14*100000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="6" xr3:uid="{08D8C7E3-7D88-435C-B063-045F43DBAF96}" name="Q5" dataDxfId="34">
-      <calculatedColumnFormula>F$22/F$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>F$63/F$14*100000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="7" xr3:uid="{46171698-FBF5-4FB0-A23B-97ACF91645E1}" name="Total" dataDxfId="33">
-      <calculatedColumnFormula>G$22/G$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>G$63/G$14*100000</calculatedColumnFormula>
     </tableColumn>
   </tableColumns>
   <tableStyleInfo name="Data-style" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
@@ -5852,7 +5863,7 @@
     <tableColumn id="1" xr3:uid="{BE65415D-B247-4ECA-88B8-35DB87E72E3C}" name="Metrics" dataDxfId="28"/>
     <tableColumn id="2" xr3:uid="{2CBE52C0-4454-44A6-9857-A82D73695559}" name="Q1" dataDxfId="27"/>
     <tableColumn id="3" xr3:uid="{67ED8C2E-6FFF-4792-8C0A-59FED451083C}" name="Q2" dataDxfId="26">
-      <calculatedColumnFormula>C$22/C$14*100000</calculatedColumnFormula>
+      <calculatedColumnFormula>C$63/C$14*100000</calculatedColumnFormula>
     </tableColumn>
     <tableColumn id="4" xr3:uid="{ECCDC4A7-53F6-4DBF-AA8F-0A29A7A98ACA}" name="Q3" dataDxfId="25"/>
     <tableColumn id="5" xr3:uid="{22786806-2BB1-4ED2-BCD5-4E7190DC3E9E}" name="Q4" dataDxfId="24"/>
@@ -6093,37 +6104,61 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{154F5DCC-65CD-4A30-A6E1-F945FCCE9B53}">
-  <dimension ref="A1:I39"/>
+  <dimension ref="A1:I66"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L38" sqref="L38"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29.7109375" customWidth="1"/>
-    <col min="2" max="2" width="14.5703125" customWidth="1"/>
-    <col min="3" max="3" width="12.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="13.5703125" customWidth="1"/>
-    <col min="6" max="6" width="13.85546875" customWidth="1"/>
-    <col min="7" max="7" width="14" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.7109375" customWidth="1"/>
+    <col min="3" max="7" width="12.7109375" customWidth="1"/>
     <col min="9" max="9" width="12.5703125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" ht="21" x14ac:dyDescent="0.35">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:9" ht="28.5" x14ac:dyDescent="0.45">
+      <c r="A1" s="40" t="s">
         <v>30</v>
       </c>
+      <c r="B1" s="40"/>
+      <c r="C1" s="40"/>
+      <c r="D1" s="40"/>
+      <c r="E1" s="40"/>
+      <c r="F1" s="40"/>
+      <c r="G1" s="40"/>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="41" t="s">
         <v>37</v>
       </c>
+      <c r="B2" s="41"/>
+      <c r="C2" s="41"/>
+      <c r="D2" s="41"/>
+      <c r="E2" s="41"/>
+      <c r="F2" s="41"/>
+      <c r="G2" s="41"/>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="42">
         <v>45995</v>
       </c>
+      <c r="B3" s="42"/>
+      <c r="C3" s="42"/>
+      <c r="D3" s="42"/>
+      <c r="E3" s="42"/>
+      <c r="F3" s="42"/>
+      <c r="G3" s="42"/>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A4" s="39"/>
+      <c r="B4" s="39"/>
+      <c r="C4" s="39"/>
+      <c r="D4" s="39"/>
+      <c r="E4" s="39"/>
+      <c r="F4" s="39"/>
+      <c r="G4" s="39"/>
     </row>
     <row r="5" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
       <c r="A5" s="5" t="s">
@@ -6131,677 +6166,686 @@
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="7" t="s">
+      <c r="A6" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B6" s="8" t="s">
+      <c r="B6" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C6" s="8" t="s">
+      <c r="C6" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D6" s="8" t="s">
+      <c r="D6" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E6" s="8" t="s">
+      <c r="E6" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F6" s="8" t="s">
+      <c r="F6" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G6" s="8" t="s">
+      <c r="G6" s="7" t="s">
         <v>5</v>
       </c>
       <c r="I6" s="4"/>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="10" t="s">
+      <c r="A7" s="9" t="s">
         <v>6</v>
       </c>
-      <c r="B7" s="11">
-        <v>0</v>
-      </c>
-      <c r="C7" s="35">
+      <c r="B7" s="10">
+        <v>0</v>
+      </c>
+      <c r="C7" s="34">
         <v>6245.56</v>
       </c>
-      <c r="D7" s="35">
+      <c r="D7" s="34">
         <v>172.23</v>
       </c>
-      <c r="E7" s="35">
+      <c r="E7" s="34">
         <v>6186.75</v>
       </c>
-      <c r="F7" s="35">
+      <c r="F7" s="34">
         <v>3390.46</v>
       </c>
-      <c r="G7" s="38">
+      <c r="G7" s="37">
         <f>SUM(B7:F7)</f>
         <v>15995</v>
       </c>
       <c r="I7" s="3"/>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="10" t="s">
+      <c r="A8" s="9" t="s">
         <v>7</v>
       </c>
-      <c r="B8" s="11">
-        <v>0</v>
-      </c>
-      <c r="C8" s="34">
-        <v>0</v>
-      </c>
-      <c r="D8" s="34">
+      <c r="B8" s="10">
+        <v>0</v>
+      </c>
+      <c r="C8" s="33">
+        <v>0</v>
+      </c>
+      <c r="D8" s="33">
         <v>171000</v>
       </c>
-      <c r="E8" s="34">
+      <c r="E8" s="33">
         <v>171000</v>
       </c>
-      <c r="F8" s="34">
-        <v>0</v>
-      </c>
-      <c r="G8" s="37">
+      <c r="F8" s="33">
+        <v>0</v>
+      </c>
+      <c r="G8" s="36">
         <f t="shared" ref="G8:G13" si="0">SUM(B8:F8)</f>
         <v>342000</v>
       </c>
       <c r="I8" s="3"/>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="10" t="s">
+      <c r="A9" s="9" t="s">
         <v>8</v>
       </c>
-      <c r="B9" s="11">
-        <v>0</v>
-      </c>
-      <c r="C9" s="34">
-        <v>0</v>
-      </c>
-      <c r="D9" s="34">
-        <v>0</v>
-      </c>
-      <c r="E9" s="34">
-        <v>0</v>
-      </c>
-      <c r="F9" s="34">
-        <v>0</v>
-      </c>
-      <c r="G9" s="37">
+      <c r="B9" s="10">
+        <v>0</v>
+      </c>
+      <c r="C9" s="33">
+        <v>0</v>
+      </c>
+      <c r="D9" s="33">
+        <v>0</v>
+      </c>
+      <c r="E9" s="33">
+        <v>0</v>
+      </c>
+      <c r="F9" s="33">
+        <v>0</v>
+      </c>
+      <c r="G9" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I9" s="3"/>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="10" t="s">
+      <c r="A10" s="9" t="s">
         <v>9</v>
       </c>
-      <c r="B10" s="11">
-        <v>0</v>
-      </c>
-      <c r="C10" s="34">
-        <v>0</v>
-      </c>
-      <c r="D10" s="34">
-        <v>0</v>
-      </c>
-      <c r="E10" s="34">
-        <v>0</v>
-      </c>
-      <c r="F10" s="34">
-        <v>0</v>
-      </c>
-      <c r="G10" s="37">
+      <c r="B10" s="10">
+        <v>0</v>
+      </c>
+      <c r="C10" s="33">
+        <v>0</v>
+      </c>
+      <c r="D10" s="33">
+        <v>0</v>
+      </c>
+      <c r="E10" s="33">
+        <v>0</v>
+      </c>
+      <c r="F10" s="33">
+        <v>0</v>
+      </c>
+      <c r="G10" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I10" s="3"/>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="10" t="s">
+      <c r="A11" s="9" t="s">
         <v>10</v>
       </c>
-      <c r="B11" s="11">
-        <v>0</v>
-      </c>
-      <c r="C11" s="34">
-        <v>0</v>
-      </c>
-      <c r="D11" s="34">
-        <v>0</v>
-      </c>
-      <c r="E11" s="34">
-        <v>0</v>
-      </c>
-      <c r="F11" s="34">
-        <v>0</v>
-      </c>
-      <c r="G11" s="37">
+      <c r="B11" s="10">
+        <v>0</v>
+      </c>
+      <c r="C11" s="33">
+        <v>0</v>
+      </c>
+      <c r="D11" s="33">
+        <v>0</v>
+      </c>
+      <c r="E11" s="33">
+        <v>0</v>
+      </c>
+      <c r="F11" s="33">
+        <v>0</v>
+      </c>
+      <c r="G11" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
       <c r="I11" s="3"/>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="10" t="s">
+      <c r="A12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="B12" s="11">
-        <v>0</v>
-      </c>
-      <c r="C12" s="34">
-        <v>0</v>
-      </c>
-      <c r="D12" s="34">
-        <v>0</v>
-      </c>
-      <c r="E12" s="34">
-        <v>0</v>
-      </c>
-      <c r="F12" s="34">
-        <v>0</v>
-      </c>
-      <c r="G12" s="37">
+      <c r="B12" s="10">
+        <v>0</v>
+      </c>
+      <c r="C12" s="33">
+        <v>0</v>
+      </c>
+      <c r="D12" s="33">
+        <v>0</v>
+      </c>
+      <c r="E12" s="33">
+        <v>0</v>
+      </c>
+      <c r="F12" s="33">
+        <v>0</v>
+      </c>
+      <c r="G12" s="36">
         <f t="shared" si="0"/>
         <v>0</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="10" t="s">
+      <c r="A13" s="9" t="s">
         <v>12</v>
       </c>
-      <c r="B13" s="11">
-        <v>0</v>
-      </c>
-      <c r="C13" s="34">
+      <c r="B13" s="10">
+        <v>0</v>
+      </c>
+      <c r="C13" s="33">
         <v>624.55999999999995</v>
       </c>
-      <c r="D13" s="34">
+      <c r="D13" s="33">
         <v>17117.22</v>
       </c>
-      <c r="E13" s="34">
+      <c r="E13" s="33">
         <v>15188.67</v>
       </c>
-      <c r="F13" s="34">
+      <c r="F13" s="33">
         <v>338.55</v>
       </c>
-      <c r="G13" s="37">
+      <c r="G13" s="36">
         <f t="shared" si="0"/>
         <v>33269.000000000007</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="13" t="s">
+      <c r="A14" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="B14" s="14">
+      <c r="B14" s="13">
         <f>SUM(B7:B13)</f>
         <v>0</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="35">
         <f>SUM(C7:C13)</f>
         <v>6870.1200000000008</v>
       </c>
-      <c r="D14" s="36">
+      <c r="D14" s="35">
         <f>SUM(D7:D13)</f>
         <v>188289.45</v>
       </c>
-      <c r="E14" s="36">
+      <c r="E14" s="35">
         <f>SUM(E7:E13)</f>
         <v>192375.42</v>
       </c>
-      <c r="F14" s="36">
+      <c r="F14" s="35">
         <f>SUM(F7:F13)</f>
         <v>3729.01</v>
       </c>
-      <c r="G14" s="39">
+      <c r="G14" s="38">
         <f ca="1">SUM(Spending[[#This Row],[Q2]:[Total]])</f>
         <v>391264</v>
       </c>
     </row>
-    <row r="16" spans="1:9" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A16" s="5" t="s">
+    <row r="27" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="28" spans="1:7" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="5" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="29" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B29" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C29" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D29" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E29" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F29" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G29" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="30" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A30" s="9" t="s">
+        <v>23</v>
+      </c>
+      <c r="B30" s="19" t="s">
+        <v>34</v>
+      </c>
+      <c r="C30" s="20">
+        <f>C$63/C$14*100000</f>
+        <v>29.111573014736276</v>
+      </c>
+      <c r="D30" s="21">
+        <f>D$63/D$14*100000</f>
+        <v>0</v>
+      </c>
+      <c r="E30" s="21">
+        <f>E$63/E$14*100000</f>
+        <v>0</v>
+      </c>
+      <c r="F30" s="21">
+        <f>F$63/F$14*100000</f>
+        <v>0</v>
+      </c>
+      <c r="G30" s="22">
+        <f ca="1">G$63/G$14*100000</f>
+        <v>0.51116381778032216</v>
+      </c>
+    </row>
+    <row r="31" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A31" s="9" t="s">
+        <v>24</v>
+      </c>
+      <c r="B31" s="23">
+        <v>0</v>
+      </c>
+      <c r="C31" s="10">
+        <f>C14/C63</f>
+        <v>3435.0600000000004</v>
+      </c>
+      <c r="D31" s="23">
+        <v>0</v>
+      </c>
+      <c r="E31" s="23">
+        <v>0</v>
+      </c>
+      <c r="F31" s="23">
+        <v>0</v>
+      </c>
+      <c r="G31" s="24">
+        <f ca="1">G14/G63</f>
+        <v>195632</v>
+      </c>
+    </row>
+    <row r="32" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A32" s="9" t="s">
+        <v>25</v>
+      </c>
+      <c r="B32" s="23">
+        <v>0</v>
+      </c>
+      <c r="C32" s="25">
+        <f>C14/C60</f>
+        <v>85.876500000000007</v>
+      </c>
+      <c r="D32" s="25">
+        <v>0</v>
+      </c>
+      <c r="E32" s="25">
+        <f>E14/E60</f>
+        <v>192375.42</v>
+      </c>
+      <c r="F32" s="25">
+        <f>F14/F60</f>
+        <v>3729.01</v>
+      </c>
+      <c r="G32" s="26">
+        <f ca="1">G14/G60</f>
+        <v>4771.5121951219517</v>
+      </c>
+    </row>
+    <row r="33" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A33" s="16" t="s">
+        <v>26</v>
+      </c>
+      <c r="B33" s="27">
+        <v>0</v>
+      </c>
+      <c r="C33" s="28">
+        <f>C14/C61</f>
+        <v>5.0716215617664</v>
+      </c>
+      <c r="D33" s="28">
+        <v>0</v>
+      </c>
+      <c r="E33" s="28">
+        <f>E14/E61</f>
+        <v>4386.1244870041046</v>
+      </c>
+      <c r="F33" s="28">
+        <f>F14/F61</f>
+        <v>46.618452306538323</v>
+      </c>
+      <c r="G33" s="29">
+        <f ca="1">G14/G61</f>
+        <v>264.64114929623196</v>
+      </c>
+    </row>
+    <row r="34" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="35" spans="1:7" hidden="1" x14ac:dyDescent="0.25"/>
+    <row r="36" spans="1:7" ht="18.75" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A36" s="5" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="37" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="6" t="s">
+        <v>22</v>
+      </c>
+      <c r="B37" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C37" s="7" t="s">
+        <v>3</v>
+      </c>
+      <c r="D37" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="E37" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="F37" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="G37" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="38" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A38" s="9" t="s">
+        <v>28</v>
+      </c>
+      <c r="B38" s="21">
+        <v>0</v>
+      </c>
+      <c r="C38" s="21">
+        <f>C63/C59</f>
+        <v>0.22222222222222221</v>
+      </c>
+      <c r="D38" s="21">
+        <f>D63/D59</f>
+        <v>0</v>
+      </c>
+      <c r="E38" s="21">
+        <f>E63/E59</f>
+        <v>0</v>
+      </c>
+      <c r="F38" s="21">
+        <f>F63/F59</f>
+        <v>0</v>
+      </c>
+      <c r="G38" s="30">
+        <f>G63/G59</f>
+        <v>7.6923076923076927E-2</v>
+      </c>
+    </row>
+    <row r="39" spans="1:7" hidden="1" x14ac:dyDescent="0.25">
+      <c r="A39" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="B39" s="31">
+        <v>0</v>
+      </c>
+      <c r="C39" s="31">
+        <f>C61/C60</f>
+        <v>16.932749999999999</v>
+      </c>
+      <c r="D39" s="31">
+        <v>0</v>
+      </c>
+      <c r="E39" s="31">
+        <f>E61/E60</f>
+        <v>43.86</v>
+      </c>
+      <c r="F39" s="31">
+        <f>F61/F60</f>
+        <v>79.989999999999995</v>
+      </c>
+      <c r="G39" s="32">
+        <f>G61/G60</f>
+        <v>18.03012195121951</v>
+      </c>
+    </row>
+    <row r="57" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="A57" s="5" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" s="7" t="s">
+    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A58" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="B17" s="8" t="s">
+      <c r="B58" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C17" s="8" t="s">
+      <c r="C58" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D17" s="8" t="s">
+      <c r="D58" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E17" s="8" t="s">
+      <c r="E58" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F17" s="8" t="s">
+      <c r="F58" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G17" s="9" t="s">
+      <c r="G58" s="8" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" s="10" t="s">
+    <row r="59" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A59" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B18" s="15">
-        <v>0</v>
-      </c>
-      <c r="C18" s="15">
+      <c r="B59" s="14">
+        <v>0</v>
+      </c>
+      <c r="C59" s="14">
         <v>9</v>
       </c>
-      <c r="D18" s="15">
+      <c r="D59" s="14">
         <v>1</v>
       </c>
-      <c r="E18" s="15">
+      <c r="E59" s="14">
         <v>8</v>
       </c>
-      <c r="F18" s="15">
+      <c r="F59" s="14">
         <v>8</v>
       </c>
-      <c r="G18" s="16">
+      <c r="G59" s="15">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>26</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="10" t="s">
+    <row r="60" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A60" s="9" t="s">
         <v>15</v>
       </c>
-      <c r="B19" s="15">
-        <v>0</v>
-      </c>
-      <c r="C19" s="15">
+      <c r="B60" s="14">
+        <v>0</v>
+      </c>
+      <c r="C60" s="14">
         <v>80</v>
       </c>
-      <c r="D19" s="15">
-        <v>0</v>
-      </c>
-      <c r="E19" s="15">
+      <c r="D60" s="14">
+        <v>0</v>
+      </c>
+      <c r="E60" s="14">
         <v>1</v>
       </c>
-      <c r="F19" s="15">
+      <c r="F60" s="14">
         <v>1</v>
       </c>
-      <c r="G19" s="16">
+      <c r="G60" s="15">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>82</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="10" t="s">
+    <row r="61" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A61" s="9" t="s">
         <v>16</v>
       </c>
-      <c r="B20" s="11">
-        <v>0</v>
-      </c>
-      <c r="C20" s="11">
+      <c r="B61" s="10">
+        <v>0</v>
+      </c>
+      <c r="C61" s="10">
         <v>1354.62</v>
       </c>
-      <c r="D20" s="11">
-        <v>0</v>
-      </c>
-      <c r="E20" s="11">
+      <c r="D61" s="10">
+        <v>0</v>
+      </c>
+      <c r="E61" s="10">
         <v>43.86</v>
       </c>
-      <c r="F20" s="11">
+      <c r="F61" s="10">
         <v>79.989999999999995</v>
       </c>
-      <c r="G20" s="12">
+      <c r="G61" s="11">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>1478.4699999999998</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="10" t="s">
+    <row r="62" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A62" s="9" t="s">
         <v>17</v>
       </c>
-      <c r="B21" s="15">
-        <v>0</v>
-      </c>
-      <c r="C21" s="15">
+      <c r="B62" s="14">
+        <v>0</v>
+      </c>
+      <c r="C62" s="14">
         <v>7</v>
       </c>
-      <c r="D21" s="15">
-        <v>0</v>
-      </c>
-      <c r="E21" s="15">
+      <c r="D62" s="14">
+        <v>0</v>
+      </c>
+      <c r="E62" s="14">
         <v>2</v>
       </c>
-      <c r="F21" s="15">
+      <c r="F62" s="14">
         <v>1</v>
       </c>
-      <c r="G21" s="16">
+      <c r="G62" s="15">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="10" t="s">
+    <row r="63" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A63" s="9" t="s">
         <v>18</v>
       </c>
-      <c r="B22" s="15">
-        <v>0</v>
-      </c>
-      <c r="C22" s="15">
+      <c r="B63" s="14">
+        <v>0</v>
+      </c>
+      <c r="C63" s="14">
         <v>2</v>
       </c>
-      <c r="D22" s="15">
-        <v>0</v>
-      </c>
-      <c r="E22" s="15">
-        <v>0</v>
-      </c>
-      <c r="F22" s="15">
-        <v>0</v>
-      </c>
-      <c r="G22" s="16">
+      <c r="D63" s="14">
+        <v>0</v>
+      </c>
+      <c r="E63" s="14">
+        <v>0</v>
+      </c>
+      <c r="F63" s="14">
+        <v>0</v>
+      </c>
+      <c r="G63" s="15">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A23" s="10" t="s">
+    <row r="64" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A64" s="9" t="s">
         <v>19</v>
       </c>
-      <c r="B23" s="15">
-        <v>0</v>
-      </c>
-      <c r="C23" s="15">
+      <c r="B64" s="14">
+        <v>0</v>
+      </c>
+      <c r="C64" s="14">
         <v>3</v>
       </c>
-      <c r="D23" s="15">
-        <v>0</v>
-      </c>
-      <c r="E23" s="15">
+      <c r="D64" s="14">
+        <v>0</v>
+      </c>
+      <c r="E64" s="14">
         <v>1</v>
       </c>
-      <c r="F23" s="15">
+      <c r="F64" s="14">
         <v>1</v>
       </c>
-      <c r="G23" s="16">
+      <c r="G64" s="15">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>5</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A24" s="10" t="s">
+    <row r="65" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A65" s="9" t="s">
         <v>20</v>
       </c>
-      <c r="B24" s="15">
-        <v>0</v>
-      </c>
-      <c r="C24" s="15">
-        <v>0</v>
-      </c>
-      <c r="D24" s="15">
-        <v>0</v>
-      </c>
-      <c r="E24" s="15">
+      <c r="B65" s="14">
+        <v>0</v>
+      </c>
+      <c r="C65" s="14">
+        <v>0</v>
+      </c>
+      <c r="D65" s="14">
+        <v>0</v>
+      </c>
+      <c r="E65" s="14">
         <v>1</v>
       </c>
-      <c r="F24" s="15">
-        <v>0</v>
-      </c>
-      <c r="G24" s="16">
+      <c r="F65" s="14">
+        <v>0</v>
+      </c>
+      <c r="G65" s="15">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>1</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A25" s="17" t="s">
+    <row r="66" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A66" s="16" t="s">
         <v>33</v>
       </c>
-      <c r="B25" s="18">
-        <v>0</v>
-      </c>
-      <c r="C25" s="18">
+      <c r="B66" s="17">
+        <v>0</v>
+      </c>
+      <c r="C66" s="17">
         <v>2</v>
       </c>
-      <c r="D25" s="18">
-        <v>0</v>
-      </c>
-      <c r="E25" s="18">
-        <v>0</v>
-      </c>
-      <c r="F25" s="18">
-        <v>0</v>
-      </c>
-      <c r="G25" s="19">
+      <c r="D66" s="17">
+        <v>0</v>
+      </c>
+      <c r="E66" s="17">
+        <v>0</v>
+      </c>
+      <c r="F66" s="17">
+        <v>0</v>
+      </c>
+      <c r="G66" s="18">
         <f>SUM(Outcomes[[#This Row],[Q1]:[Q5]])</f>
         <v>2</v>
       </c>
     </row>
-    <row r="28" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A28" s="5" t="s">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A29" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B29" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C29" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D29" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E29" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F29" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G29" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="10" t="s">
-        <v>23</v>
-      </c>
-      <c r="B30" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="C30" s="21">
-        <f>C$22/C$14*100000</f>
-        <v>29.111573014736276</v>
-      </c>
-      <c r="D30" s="22">
-        <f>D$22/D$14*100000</f>
-        <v>0</v>
-      </c>
-      <c r="E30" s="22">
-        <f>E$22/E$14*100000</f>
-        <v>0</v>
-      </c>
-      <c r="F30" s="22">
-        <f>F$22/F$14*100000</f>
-        <v>0</v>
-      </c>
-      <c r="G30" s="23">
-        <f ca="1">G$22/G$14*100000</f>
-        <v>0.51116381778032216</v>
-      </c>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="10" t="s">
-        <v>24</v>
-      </c>
-      <c r="B31" s="24">
-        <v>0</v>
-      </c>
-      <c r="C31" s="11">
-        <f>C14/C22</f>
-        <v>3435.0600000000004</v>
-      </c>
-      <c r="D31" s="24">
-        <v>0</v>
-      </c>
-      <c r="E31" s="24">
-        <v>0</v>
-      </c>
-      <c r="F31" s="24">
-        <v>0</v>
-      </c>
-      <c r="G31" s="25">
-        <f ca="1">G14/G22</f>
-        <v>195632</v>
-      </c>
-    </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A32" s="10" t="s">
-        <v>25</v>
-      </c>
-      <c r="B32" s="24">
-        <v>0</v>
-      </c>
-      <c r="C32" s="26">
-        <f>C14/C19</f>
-        <v>85.876500000000007</v>
-      </c>
-      <c r="D32" s="26">
-        <v>0</v>
-      </c>
-      <c r="E32" s="26">
-        <f>E14/E19</f>
-        <v>192375.42</v>
-      </c>
-      <c r="F32" s="26">
-        <f>F14/F19</f>
-        <v>3729.01</v>
-      </c>
-      <c r="G32" s="27">
-        <f ca="1">G14/G19</f>
-        <v>4771.5121951219517</v>
-      </c>
-    </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A33" s="17" t="s">
-        <v>26</v>
-      </c>
-      <c r="B33" s="28">
-        <v>0</v>
-      </c>
-      <c r="C33" s="29">
-        <f>C14/C20</f>
-        <v>5.0716215617664</v>
-      </c>
-      <c r="D33" s="29">
-        <v>0</v>
-      </c>
-      <c r="E33" s="29">
-        <f>E14/E20</f>
-        <v>4386.1244870041046</v>
-      </c>
-      <c r="F33" s="29">
-        <f>F14/F20</f>
-        <v>46.618452306538323</v>
-      </c>
-      <c r="G33" s="30">
-        <f ca="1">G14/G20</f>
-        <v>264.64114929623196</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" ht="18.75" x14ac:dyDescent="0.3">
-      <c r="A36" s="5" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="37" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A37" s="7" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>2</v>
-      </c>
-      <c r="C37" s="8" t="s">
-        <v>3</v>
-      </c>
-      <c r="D37" s="8" t="s">
-        <v>4</v>
-      </c>
-      <c r="E37" s="8" t="s">
-        <v>31</v>
-      </c>
-      <c r="F37" s="8" t="s">
-        <v>32</v>
-      </c>
-      <c r="G37" s="9" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A38" s="10" t="s">
-        <v>28</v>
-      </c>
-      <c r="B38" s="22">
-        <v>0</v>
-      </c>
-      <c r="C38" s="22">
-        <f>C22/C18</f>
-        <v>0.22222222222222221</v>
-      </c>
-      <c r="D38" s="22">
-        <f>D22/D18</f>
-        <v>0</v>
-      </c>
-      <c r="E38" s="22">
-        <f>E22/E18</f>
-        <v>0</v>
-      </c>
-      <c r="F38" s="22">
-        <f>F22/F18</f>
-        <v>0</v>
-      </c>
-      <c r="G38" s="31">
-        <f>G22/G18</f>
-        <v>7.6923076923076927E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A39" s="17" t="s">
-        <v>29</v>
-      </c>
-      <c r="B39" s="32">
-        <v>0</v>
-      </c>
-      <c r="C39" s="32">
-        <f>C20/C19</f>
-        <v>16.932749999999999</v>
-      </c>
-      <c r="D39" s="32">
-        <v>0</v>
-      </c>
-      <c r="E39" s="32">
-        <f>E20/E19</f>
-        <v>43.86</v>
-      </c>
-      <c r="F39" s="32">
-        <f>F20/F19</f>
-        <v>79.989999999999995</v>
-      </c>
-      <c r="G39" s="33">
-        <f>G20/G19</f>
-        <v>18.03012195121951</v>
-      </c>
-    </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <mergeCells count="3">
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A3:G3"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="4">
-    <tablePart r:id="rId2"/>
     <tablePart r:id="rId3"/>
     <tablePart r:id="rId4"/>
     <tablePart r:id="rId5"/>
+    <tablePart r:id="rId6"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6813,42 +6857,48 @@
   </sheetPr>
   <dimension ref="A1:K6"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H1" sqref="H1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28" customWidth="1"/>
-    <col min="2" max="2" width="11" customWidth="1"/>
-    <col min="3" max="3" width="11.85546875" customWidth="1"/>
-    <col min="4" max="4" width="12.42578125" customWidth="1"/>
-    <col min="5" max="5" width="13.5703125" customWidth="1"/>
+    <col min="1" max="1" width="28.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="10" customWidth="1"/>
+    <col min="3" max="7" width="12.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:11" ht="24" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>21</v>
       </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
       <c r="H2" s="1"/>
@@ -6857,25 +6907,25 @@
       <c r="K2" s="1"/>
     </row>
     <row r="3" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>23</v>
       </c>
-      <c r="B3" s="20" t="s">
+      <c r="B3" s="19" t="s">
         <v>34</v>
       </c>
-      <c r="C3" s="21">
+      <c r="C3" s="20">
         <v>29.111573014736276</v>
       </c>
-      <c r="D3" s="22">
-        <v>0</v>
-      </c>
-      <c r="E3" s="22">
-        <v>0</v>
-      </c>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="23">
+      <c r="D3" s="21">
+        <v>0</v>
+      </c>
+      <c r="E3" s="21">
+        <v>0</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
+      <c r="G3" s="22">
         <v>0.51116381778032216</v>
       </c>
       <c r="H3" s="2"/>
@@ -6884,25 +6934,25 @@
       <c r="K3" s="2"/>
     </row>
     <row r="4" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="10" t="s">
+      <c r="A4" s="9" t="s">
         <v>36</v>
       </c>
-      <c r="B4" s="24">
-        <v>0</v>
-      </c>
-      <c r="C4" s="11">
+      <c r="B4" s="23">
+        <v>0</v>
+      </c>
+      <c r="C4" s="10">
         <v>3435.0600000000004</v>
       </c>
-      <c r="D4" s="24">
-        <v>0</v>
-      </c>
-      <c r="E4" s="24">
-        <v>0</v>
-      </c>
-      <c r="F4" s="24">
-        <v>0</v>
-      </c>
-      <c r="G4" s="25">
+      <c r="D4" s="23">
+        <v>0</v>
+      </c>
+      <c r="E4" s="23">
+        <v>0</v>
+      </c>
+      <c r="F4" s="23">
+        <v>0</v>
+      </c>
+      <c r="G4" s="24">
         <v>195632</v>
       </c>
       <c r="H4" s="2"/>
@@ -6911,25 +6961,25 @@
       <c r="K4" s="2"/>
     </row>
     <row r="5" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="10" t="s">
+      <c r="A5" s="9" t="s">
         <v>35</v>
       </c>
-      <c r="B5" s="24">
-        <v>0</v>
-      </c>
-      <c r="C5" s="26">
+      <c r="B5" s="23">
+        <v>0</v>
+      </c>
+      <c r="C5" s="25">
         <v>85.876500000000007</v>
       </c>
-      <c r="D5" s="26">
-        <v>0</v>
-      </c>
-      <c r="E5" s="26">
+      <c r="D5" s="25">
+        <v>0</v>
+      </c>
+      <c r="E5" s="25">
         <v>192375.42</v>
       </c>
-      <c r="F5" s="26">
+      <c r="F5" s="25">
         <v>3729.01</v>
       </c>
-      <c r="G5" s="27">
+      <c r="G5" s="26">
         <v>4771.5121951219517</v>
       </c>
       <c r="H5" s="2"/>
@@ -6938,25 +6988,25 @@
       <c r="K5" s="2"/>
     </row>
     <row r="6" spans="1:11" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
+      <c r="A6" s="16" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="28">
-        <v>0</v>
-      </c>
-      <c r="C6" s="29">
+      <c r="B6" s="27">
+        <v>0</v>
+      </c>
+      <c r="C6" s="28">
         <v>5.0716215617664</v>
       </c>
-      <c r="D6" s="29">
-        <v>0</v>
-      </c>
-      <c r="E6" s="29">
+      <c r="D6" s="28">
+        <v>0</v>
+      </c>
+      <c r="E6" s="28">
         <v>4386.1244870041046</v>
       </c>
-      <c r="F6" s="29">
+      <c r="F6" s="28">
         <v>46.618452306538323</v>
       </c>
-      <c r="G6" s="30">
+      <c r="G6" s="29">
         <v>264.64114929623196</v>
       </c>
       <c r="H6" s="2"/>
@@ -6965,10 +7015,14 @@
       <c r="K6" s="2"/>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
@@ -6981,97 +7035,105 @@
   <dimension ref="A1:G4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="I24" sqref="I24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="29" customWidth="1"/>
-    <col min="2" max="2" width="11.28515625" customWidth="1"/>
-    <col min="3" max="3" width="10.42578125" customWidth="1"/>
-    <col min="4" max="4" width="9.85546875" customWidth="1"/>
-    <col min="5" max="5" width="9.7109375" customWidth="1"/>
+    <col min="1" max="1" width="28.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="11.140625" customWidth="1"/>
+    <col min="3" max="7" width="12.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="24" x14ac:dyDescent="0.4">
-      <c r="A1" s="40" t="s">
+      <c r="A1" s="43" t="s">
         <v>27</v>
       </c>
+      <c r="B1" s="43"/>
+      <c r="C1" s="43"/>
+      <c r="D1" s="43"/>
+      <c r="E1" s="43"/>
+      <c r="F1" s="43"/>
+      <c r="G1" s="43"/>
     </row>
     <row r="2" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="B2" s="8" t="s">
+      <c r="B2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C2" s="8" t="s">
+      <c r="C2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="D2" s="8" t="s">
+      <c r="D2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="E2" s="8" t="s">
+      <c r="E2" s="7" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="8" t="s">
+      <c r="F2" s="7" t="s">
         <v>32</v>
       </c>
-      <c r="G2" s="9" t="s">
+      <c r="G2" s="8" t="s">
         <v>5</v>
       </c>
     </row>
     <row r="3" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A3" s="10" t="s">
+      <c r="A3" s="9" t="s">
         <v>28</v>
       </c>
-      <c r="B3" s="22">
-        <v>0</v>
-      </c>
-      <c r="C3" s="22">
+      <c r="B3" s="21">
+        <v>0</v>
+      </c>
+      <c r="C3" s="21">
         <v>0.22222222222222221</v>
       </c>
-      <c r="D3" s="22">
-        <v>0</v>
-      </c>
-      <c r="E3" s="22">
-        <v>0</v>
-      </c>
-      <c r="F3" s="22">
-        <v>0</v>
-      </c>
-      <c r="G3" s="31">
+      <c r="D3" s="21">
+        <v>0</v>
+      </c>
+      <c r="E3" s="21">
+        <v>0</v>
+      </c>
+      <c r="F3" s="21">
+        <v>0</v>
+      </c>
+      <c r="G3" s="30">
         <v>7.6923076923076927E-2</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="22.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="17" t="s">
+      <c r="A4" s="16" t="s">
         <v>29</v>
       </c>
-      <c r="B4" s="32">
-        <v>0</v>
-      </c>
-      <c r="C4" s="32">
+      <c r="B4" s="31">
+        <v>0</v>
+      </c>
+      <c r="C4" s="31">
         <v>16.932749999999999</v>
       </c>
-      <c r="D4" s="32">
-        <v>0</v>
-      </c>
-      <c r="E4" s="32">
+      <c r="D4" s="31">
+        <v>0</v>
+      </c>
+      <c r="E4" s="31">
         <v>43.86</v>
       </c>
-      <c r="F4" s="32">
+      <c r="F4" s="31">
         <v>79.989999999999995</v>
       </c>
-      <c r="G4" s="33">
+      <c r="G4" s="32">
         <v>18.03012195121951</v>
       </c>
     </row>
   </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <mergeCells count="1">
+    <mergeCell ref="A1:G1"/>
+  </mergeCells>
+  <pageMargins left="0.25" right="0.25" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
   <tableParts count="1">
-    <tablePart r:id="rId2"/>
+    <tablePart r:id="rId3"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>